<commit_message>
Added multithreading and various optimizations
</commit_message>
<xml_diff>
--- a/Testing Files/Determiner Test Files/HatcoMLSDataTestingSmall.xlsx
+++ b/Testing Files/Determiner Test Files/HatcoMLSDataTestingSmall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\HatcoMarketShareHelper\Testing Files\Determiner Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F076CC2-62A1-4791-A103-9B9F31AECA22}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A57803-4F90-45AA-9087-10DE231B29C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="490">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -1498,30 +1498,6 @@
   </si>
   <si>
     <t>613 Ross Road</t>
-  </si>
-  <si>
-    <t>Likely Closed</t>
-  </si>
-  <si>
-    <t>Escrow Officer</t>
-  </si>
-  <si>
-    <t>did not close</t>
-  </si>
-  <si>
-    <t>Phyllis Alexander</t>
-  </si>
-  <si>
-    <t>Tiffany Minnish</t>
-  </si>
-  <si>
-    <t>Kristy Kyle</t>
-  </si>
-  <si>
-    <t>Liz Rigney</t>
-  </si>
-  <si>
-    <t>Sherry Dixon</t>
   </si>
 </sst>
 </file>
@@ -2368,22 +2344,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M126"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2417,14 +2393,8 @@
       <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>196</v>
       </c>
@@ -2455,11 +2425,8 @@
       <c r="J2" s="2">
         <v>135750</v>
       </c>
-      <c r="K2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -2490,17 +2457,8 @@
       <c r="J3" s="2">
         <v>105000</v>
       </c>
-      <c r="K3">
-        <v>20182608</v>
-      </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -2531,14 +2489,8 @@
       <c r="J4" s="2">
         <v>233000</v>
       </c>
-      <c r="K4">
-        <v>20182762</v>
-      </c>
-      <c r="M4" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -2569,11 +2521,8 @@
       <c r="J5" s="2">
         <v>365000</v>
       </c>
-      <c r="K5" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -2604,11 +2553,8 @@
       <c r="J6" s="2">
         <v>269000</v>
       </c>
-      <c r="K6" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2639,11 +2585,8 @@
       <c r="J7" s="2">
         <v>86500</v>
       </c>
-      <c r="K7" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -2674,11 +2617,8 @@
       <c r="J8" s="2">
         <v>151800</v>
       </c>
-      <c r="K8" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -2709,11 +2649,8 @@
       <c r="J9" s="2">
         <v>179500</v>
       </c>
-      <c r="K9" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2744,11 +2681,8 @@
       <c r="J10" s="2">
         <v>165000</v>
       </c>
-      <c r="K10" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -2779,11 +2713,8 @@
       <c r="J11" s="2">
         <v>135000</v>
       </c>
-      <c r="K11" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -2814,11 +2745,8 @@
       <c r="J12" s="2">
         <v>321500</v>
       </c>
-      <c r="K12" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -2849,11 +2777,8 @@
       <c r="J13" s="2">
         <v>186000</v>
       </c>
-      <c r="K13" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -2884,14 +2809,8 @@
       <c r="J14" s="2">
         <v>235000</v>
       </c>
-      <c r="K14">
-        <v>20182543</v>
-      </c>
-      <c r="M14" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2922,14 +2841,8 @@
       <c r="J15" s="2">
         <v>512000</v>
       </c>
-      <c r="K15">
-        <v>20182805</v>
-      </c>
-      <c r="M15" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>236</v>
       </c>
@@ -2960,14 +2873,8 @@
       <c r="J16" s="2">
         <v>82900</v>
       </c>
-      <c r="K16">
-        <v>20182786</v>
-      </c>
-      <c r="M16" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2998,11 +2905,8 @@
       <c r="J17" s="2">
         <v>270000</v>
       </c>
-      <c r="K17" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3033,11 +2937,8 @@
       <c r="J18" s="2">
         <v>223000</v>
       </c>
-      <c r="K18" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -3068,14 +2969,8 @@
       <c r="J19" s="2">
         <v>260000</v>
       </c>
-      <c r="K19">
-        <v>20182789</v>
-      </c>
-      <c r="M19" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -3106,11 +3001,8 @@
       <c r="J20" s="2">
         <v>132000</v>
       </c>
-      <c r="K20" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -3141,11 +3033,8 @@
       <c r="J21" s="2">
         <v>51500</v>
       </c>
-      <c r="K21" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>295</v>
       </c>
@@ -3176,14 +3065,8 @@
       <c r="J22" s="2">
         <v>499900</v>
       </c>
-      <c r="K22">
-        <v>20182635</v>
-      </c>
-      <c r="M22" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>127</v>
       </c>
@@ -3214,11 +3097,8 @@
       <c r="J23" s="2">
         <v>164500</v>
       </c>
-      <c r="K23" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -3249,11 +3129,8 @@
       <c r="J24" s="2">
         <v>860000</v>
       </c>
-      <c r="K24" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -3284,17 +3161,8 @@
       <c r="J25" s="2">
         <v>245000</v>
       </c>
-      <c r="K25">
-        <v>20182703</v>
-      </c>
-      <c r="L25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M25" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -3325,11 +3193,8 @@
       <c r="J26" s="2">
         <v>95000</v>
       </c>
-      <c r="K26" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>225</v>
       </c>
@@ -3360,11 +3225,8 @@
       <c r="J27" s="2">
         <v>290000</v>
       </c>
-      <c r="K27" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3395,14 +3257,8 @@
       <c r="J28" s="2">
         <v>165000</v>
       </c>
-      <c r="K28">
-        <v>20182779</v>
-      </c>
-      <c r="M28" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3433,11 +3289,8 @@
       <c r="J29" s="2">
         <v>91000</v>
       </c>
-      <c r="K29" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>262</v>
       </c>
@@ -3468,11 +3321,8 @@
       <c r="J30" s="2">
         <v>33000</v>
       </c>
-      <c r="K30" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -3503,11 +3353,8 @@
       <c r="J31" s="2">
         <v>747000</v>
       </c>
-      <c r="K31" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -3538,11 +3385,8 @@
       <c r="J32" s="2">
         <v>245000</v>
       </c>
-      <c r="K32" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -3573,14 +3417,8 @@
       <c r="J33" s="2">
         <v>320000</v>
       </c>
-      <c r="K33">
-        <v>20192924</v>
-      </c>
-      <c r="M33" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>112</v>
       </c>
@@ -3611,11 +3449,8 @@
       <c r="J34" s="2">
         <v>376320</v>
       </c>
-      <c r="K34" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -3646,11 +3481,8 @@
       <c r="J35" s="2">
         <v>235000</v>
       </c>
-      <c r="K35" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -3681,17 +3513,8 @@
       <c r="J36" s="2">
         <v>135000</v>
       </c>
-      <c r="K36">
-        <v>20182806</v>
-      </c>
-      <c r="L36" t="b">
-        <v>1</v>
-      </c>
-      <c r="M36" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>290</v>
       </c>
@@ -3722,11 +3545,8 @@
       <c r="J37" s="2">
         <v>139900</v>
       </c>
-      <c r="K37" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -3757,14 +3577,8 @@
       <c r="J38" s="2">
         <v>197000</v>
       </c>
-      <c r="K38">
-        <v>20182836</v>
-      </c>
-      <c r="M38" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>181</v>
       </c>
@@ -3795,14 +3609,8 @@
       <c r="J39" s="2">
         <v>165400</v>
       </c>
-      <c r="K39">
-        <v>20182829</v>
-      </c>
-      <c r="M39" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -3833,11 +3641,8 @@
       <c r="J40" s="2">
         <v>63000</v>
       </c>
-      <c r="K40" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -3868,11 +3673,8 @@
       <c r="J41" s="2">
         <v>98000</v>
       </c>
-      <c r="K41" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -3903,11 +3705,8 @@
       <c r="J42" s="2">
         <v>52500</v>
       </c>
-      <c r="K42" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -3938,11 +3737,8 @@
       <c r="J43" s="2">
         <v>117500</v>
       </c>
-      <c r="K43" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -3973,11 +3769,8 @@
       <c r="J44" s="2">
         <v>535000</v>
       </c>
-      <c r="K44" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -4008,14 +3801,8 @@
       <c r="J45" s="2">
         <v>159500</v>
       </c>
-      <c r="K45">
-        <v>20190037</v>
-      </c>
-      <c r="M45" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -4046,11 +3833,8 @@
       <c r="J46" s="2">
         <v>48000</v>
       </c>
-      <c r="K46" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>213</v>
       </c>
@@ -4081,11 +3865,8 @@
       <c r="J47" s="2">
         <v>119900</v>
       </c>
-      <c r="K47" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -4116,11 +3897,8 @@
       <c r="J48" s="2">
         <v>159950</v>
       </c>
-      <c r="K48" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>254</v>
       </c>
@@ -4151,11 +3929,8 @@
       <c r="J49" s="2">
         <v>240000</v>
       </c>
-      <c r="K49" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -4186,11 +3961,8 @@
       <c r="J50" s="2">
         <v>135000</v>
       </c>
-      <c r="K50" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -4221,17 +3993,8 @@
       <c r="J51" s="2">
         <v>186500</v>
       </c>
-      <c r="K51">
-        <v>20182810</v>
-      </c>
-      <c r="L51" t="b">
-        <v>1</v>
-      </c>
-      <c r="M51" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -4262,11 +4025,8 @@
       <c r="J52" s="2">
         <v>142000</v>
       </c>
-      <c r="K52" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>288</v>
       </c>
@@ -4297,14 +4057,8 @@
       <c r="J53" s="2">
         <v>143300</v>
       </c>
-      <c r="K53">
-        <v>20182662</v>
-      </c>
-      <c r="M53" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -4335,11 +4089,8 @@
       <c r="J54" s="2">
         <v>132000</v>
       </c>
-      <c r="K54" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -4370,11 +4121,8 @@
       <c r="J55" s="2">
         <v>495000</v>
       </c>
-      <c r="K55" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -4405,11 +4153,8 @@
       <c r="J56" s="2">
         <v>155000</v>
       </c>
-      <c r="K56" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -4440,11 +4185,8 @@
       <c r="J57" s="2">
         <v>115000</v>
       </c>
-      <c r="K57" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>343</v>
       </c>
@@ -4475,14 +4217,8 @@
       <c r="J58" s="2">
         <v>414750</v>
       </c>
-      <c r="K58">
-        <v>20182761</v>
-      </c>
-      <c r="M58" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>139</v>
       </c>
@@ -4513,14 +4249,8 @@
       <c r="J59" s="2">
         <v>55000</v>
       </c>
-      <c r="K59">
-        <v>20190030</v>
-      </c>
-      <c r="M59" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>162</v>
       </c>
@@ -4551,14 +4281,8 @@
       <c r="J60" s="2">
         <v>468000</v>
       </c>
-      <c r="K60">
-        <v>20182899</v>
-      </c>
-      <c r="M60" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>140</v>
       </c>
@@ -4589,11 +4313,8 @@
       <c r="J61" s="2">
         <v>530000</v>
       </c>
-      <c r="K61" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -4624,11 +4345,8 @@
       <c r="J62" s="2">
         <v>420000</v>
       </c>
-      <c r="K62" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -4659,11 +4377,8 @@
       <c r="J63" s="2">
         <v>150000</v>
       </c>
-      <c r="K63" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -4694,11 +4409,8 @@
       <c r="J64" s="2">
         <v>525000</v>
       </c>
-      <c r="K64" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>154</v>
       </c>
@@ -4729,11 +4441,8 @@
       <c r="J65" s="2">
         <v>191425</v>
       </c>
-      <c r="K65" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>295</v>
       </c>
@@ -4764,14 +4473,8 @@
       <c r="J66" s="2">
         <v>450000</v>
       </c>
-      <c r="K66">
-        <v>20182825</v>
-      </c>
-      <c r="M66" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -4802,11 +4505,8 @@
       <c r="J67" s="2">
         <v>198000</v>
       </c>
-      <c r="K67" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -4837,11 +4537,8 @@
       <c r="J68" s="2">
         <v>265250</v>
       </c>
-      <c r="K68" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>140</v>
       </c>
@@ -4872,11 +4569,8 @@
       <c r="J69" s="2">
         <v>223000</v>
       </c>
-      <c r="K69" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>185</v>
       </c>
@@ -4907,11 +4601,8 @@
       <c r="J70" s="2">
         <v>27000</v>
       </c>
-      <c r="K70" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -4942,11 +4633,8 @@
       <c r="J71" s="2">
         <v>142900</v>
       </c>
-      <c r="K71" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>259</v>
       </c>
@@ -4977,11 +4665,8 @@
       <c r="J72" s="2">
         <v>50000</v>
       </c>
-      <c r="K72" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -5012,11 +4697,8 @@
       <c r="J73" s="2">
         <v>204500</v>
       </c>
-      <c r="K73" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -5047,11 +4729,8 @@
       <c r="J74" s="2">
         <v>133500</v>
       </c>
-      <c r="K74" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -5082,17 +4761,8 @@
       <c r="J75" s="2">
         <v>18000</v>
       </c>
-      <c r="K75">
-        <v>20182360</v>
-      </c>
-      <c r="L75" t="b">
-        <v>1</v>
-      </c>
-      <c r="M75" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>246</v>
       </c>
@@ -5123,11 +4793,8 @@
       <c r="J76" s="2">
         <v>199900</v>
       </c>
-      <c r="K76" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>51</v>
       </c>
@@ -5158,11 +4825,8 @@
       <c r="J77" s="2">
         <v>299000</v>
       </c>
-      <c r="K77" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -5193,11 +4857,8 @@
       <c r="J78" s="2">
         <v>101400</v>
       </c>
-      <c r="K78" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -5228,11 +4889,8 @@
       <c r="J79" s="2">
         <v>345000</v>
       </c>
-      <c r="K79" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -5263,11 +4921,8 @@
       <c r="J80" s="2">
         <v>50000</v>
       </c>
-      <c r="K80" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>30</v>
       </c>
@@ -5298,11 +4953,8 @@
       <c r="J81" s="2">
         <v>237500</v>
       </c>
-      <c r="K81" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>154</v>
       </c>
@@ -5333,11 +4985,8 @@
       <c r="J82" s="2">
         <v>369900</v>
       </c>
-      <c r="K82" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -5368,11 +5017,8 @@
       <c r="J83" s="2">
         <v>130000</v>
       </c>
-      <c r="K83" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>59</v>
       </c>
@@ -5403,11 +5049,8 @@
       <c r="J84" s="2">
         <v>189000</v>
       </c>
-      <c r="K84" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>56</v>
       </c>
@@ -5438,11 +5081,8 @@
       <c r="J85" s="2">
         <v>197000</v>
       </c>
-      <c r="K85" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -5473,14 +5113,8 @@
       <c r="J86" s="2">
         <v>297500</v>
       </c>
-      <c r="K86">
-        <v>20182729</v>
-      </c>
-      <c r="M86" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>109</v>
       </c>
@@ -5511,11 +5145,8 @@
       <c r="J87" s="2">
         <v>233000</v>
       </c>
-      <c r="K87" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>60</v>
       </c>
@@ -5546,11 +5177,8 @@
       <c r="J88" s="2">
         <v>307000</v>
       </c>
-      <c r="K88" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>123</v>
       </c>
@@ -5581,11 +5209,8 @@
       <c r="J89" s="2">
         <v>78000</v>
       </c>
-      <c r="K89" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>53</v>
       </c>
@@ -5616,11 +5241,8 @@
       <c r="J90" s="2">
         <v>370000</v>
       </c>
-      <c r="K90" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -5651,14 +5273,8 @@
       <c r="J91" s="2">
         <v>299000</v>
       </c>
-      <c r="K91">
-        <v>20182865</v>
-      </c>
-      <c r="M91" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>45</v>
       </c>
@@ -5689,11 +5305,8 @@
       <c r="J92" s="2">
         <v>133000</v>
       </c>
-      <c r="K92" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>402</v>
       </c>
@@ -5724,11 +5337,8 @@
       <c r="J93" s="2">
         <v>133000</v>
       </c>
-      <c r="K93" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>465</v>
       </c>
@@ -5759,14 +5369,8 @@
       <c r="J94" s="2">
         <v>169900</v>
       </c>
-      <c r="K94">
-        <v>20182852</v>
-      </c>
-      <c r="M94" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>32</v>
       </c>
@@ -5797,11 +5401,8 @@
       <c r="J95" s="2">
         <v>135000</v>
       </c>
-      <c r="K95" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>294</v>
       </c>
@@ -5832,11 +5433,8 @@
       <c r="J96" s="2">
         <v>274000</v>
       </c>
-      <c r="K96" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>129</v>
       </c>
@@ -5867,14 +5465,8 @@
       <c r="J97" s="2">
         <v>160000</v>
       </c>
-      <c r="K97">
-        <v>20182904</v>
-      </c>
-      <c r="M97" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -5905,11 +5497,8 @@
       <c r="J98" s="2">
         <v>103000</v>
       </c>
-      <c r="K98" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>75</v>
       </c>
@@ -5940,14 +5529,8 @@
       <c r="J99" s="2">
         <v>462000</v>
       </c>
-      <c r="K99">
-        <v>20182817</v>
-      </c>
-      <c r="M99" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>73</v>
       </c>
@@ -5978,11 +5561,8 @@
       <c r="J100" s="2">
         <v>280000</v>
       </c>
-      <c r="K100" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>172</v>
       </c>
@@ -6013,11 +5593,8 @@
       <c r="J101" s="2">
         <v>130000</v>
       </c>
-      <c r="K101" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>78</v>
       </c>
@@ -6048,11 +5625,8 @@
       <c r="J102" s="2">
         <v>112000</v>
       </c>
-      <c r="K102" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>72</v>
       </c>
@@ -6083,11 +5657,8 @@
       <c r="J103" s="2">
         <v>110100</v>
       </c>
-      <c r="K103" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>168</v>
       </c>
@@ -6118,17 +5689,8 @@
       <c r="J104" s="2">
         <v>139000</v>
       </c>
-      <c r="K104">
-        <v>20191942</v>
-      </c>
-      <c r="L104" t="b">
-        <v>1</v>
-      </c>
-      <c r="M104" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>53</v>
       </c>
@@ -6159,11 +5721,8 @@
       <c r="J105" s="2">
         <v>310000</v>
       </c>
-      <c r="K105" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>66</v>
       </c>
@@ -6194,14 +5753,8 @@
       <c r="J106" s="2">
         <v>126900</v>
       </c>
-      <c r="K106">
-        <v>20182874</v>
-      </c>
-      <c r="M106" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -6232,14 +5785,8 @@
       <c r="J107" s="2">
         <v>450000</v>
       </c>
-      <c r="K107">
-        <v>20182896</v>
-      </c>
-      <c r="M107" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>88</v>
       </c>
@@ -6270,11 +5817,8 @@
       <c r="J108" s="2">
         <v>164000</v>
       </c>
-      <c r="K108" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -6305,14 +5849,8 @@
       <c r="J109" s="2">
         <v>106000</v>
       </c>
-      <c r="K109">
-        <v>20190072</v>
-      </c>
-      <c r="M109" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>183</v>
       </c>
@@ -6343,11 +5881,8 @@
       <c r="J110" s="2">
         <v>145000</v>
       </c>
-      <c r="K110" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>74</v>
       </c>
@@ -6378,11 +5913,8 @@
       <c r="J111" s="2">
         <v>78000</v>
       </c>
-      <c r="K111" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>176</v>
       </c>
@@ -6413,11 +5945,8 @@
       <c r="J112" s="2">
         <v>176900</v>
       </c>
-      <c r="K112" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>32</v>
       </c>
@@ -6448,11 +5977,8 @@
       <c r="J113" s="2">
         <v>30000</v>
       </c>
-      <c r="K113" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>126</v>
       </c>
@@ -6483,14 +6009,8 @@
       <c r="J114" s="2">
         <v>353000</v>
       </c>
-      <c r="K114">
-        <v>20192925</v>
-      </c>
-      <c r="M114" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>127</v>
       </c>
@@ -6521,11 +6041,8 @@
       <c r="J115" s="2">
         <v>88400</v>
       </c>
-      <c r="K115" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>34</v>
       </c>
@@ -6556,17 +6073,8 @@
       <c r="J116" s="2">
         <v>158400</v>
       </c>
-      <c r="K116">
-        <v>20182854</v>
-      </c>
-      <c r="L116" t="b">
-        <v>1</v>
-      </c>
-      <c r="M116" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>67</v>
       </c>
@@ -6597,11 +6105,8 @@
       <c r="J117" s="2">
         <v>290000</v>
       </c>
-      <c r="K117" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>79</v>
       </c>
@@ -6632,11 +6137,8 @@
       <c r="J118" s="2">
         <v>180000</v>
       </c>
-      <c r="K118" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>53</v>
       </c>
@@ -6667,11 +6169,8 @@
       <c r="J119" s="2">
         <v>80000</v>
       </c>
-      <c r="K119" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>186</v>
       </c>
@@ -6702,11 +6201,8 @@
       <c r="J120" s="2">
         <v>75000</v>
       </c>
-      <c r="K120" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>190</v>
       </c>
@@ -6737,11 +6233,8 @@
       <c r="J121" s="2">
         <v>184900</v>
       </c>
-      <c r="K121" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -6772,11 +6265,8 @@
       <c r="J122" s="2">
         <v>405000</v>
       </c>
-      <c r="K122" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>34</v>
       </c>
@@ -6807,11 +6297,8 @@
       <c r="J123" s="2">
         <v>273000</v>
       </c>
-      <c r="K123" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>289</v>
       </c>
@@ -6842,11 +6329,8 @@
       <c r="J124" s="2">
         <v>43750</v>
       </c>
-      <c r="K124" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>50</v>
       </c>
@@ -6877,11 +6361,8 @@
       <c r="J125" s="2">
         <v>179000</v>
       </c>
-      <c r="K125" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>35</v>
       </c>
@@ -6912,12 +6393,9 @@
       <c r="J126" s="2">
         <v>232000</v>
       </c>
-      <c r="K126" t="s">
-        <v>492</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M126">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K126">
     <sortCondition ref="I2:I126"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some tweaks to prevent memory leak issue when multithreading
</commit_message>
<xml_diff>
--- a/Testing Files/Determiner Test Files/HatcoMLSDataTestingSmall.xlsx
+++ b/Testing Files/Determiner Test Files/HatcoMLSDataTestingSmall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\HatcoMarketShareHelper\Testing Files\Determiner Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B71E7E-DD7D-4176-B997-BC5445D02B71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0102E18F-7F87-49B8-9931-430C03D888E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="408" yWindow="408" windowWidth="17280" windowHeight="9036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MLSData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="498">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -1506,22 +1506,22 @@
     <t>Escrow Officer</t>
   </si>
   <si>
+    <t>Tiffany Minnish</t>
+  </si>
+  <si>
     <t>did not close</t>
   </si>
   <si>
+    <t>Phyllis Alexander</t>
+  </si>
+  <si>
+    <t>Kristy Kyle</t>
+  </si>
+  <si>
     <t>Liz Rigney</t>
   </si>
   <si>
-    <t>Phyllis Alexander</t>
-  </si>
-  <si>
     <t>Sherry Dixon</t>
-  </si>
-  <si>
-    <t>Tiffany Minnish</t>
-  </si>
-  <si>
-    <t>Kristy Kyle</t>
   </si>
 </sst>
 </file>
@@ -2371,19 +2371,19 @@
   <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="29.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>196</v>
       </c>
@@ -2456,10 +2456,10 @@
         <v>135750</v>
       </c>
       <c r="K2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -2535,10 +2535,10 @@
         <v>20182762</v>
       </c>
       <c r="M4" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -2570,10 +2570,10 @@
         <v>365000</v>
       </c>
       <c r="K5" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2646,10 +2646,10 @@
         <v>86500</v>
       </c>
       <c r="K7" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -2681,10 +2681,10 @@
         <v>151800</v>
       </c>
       <c r="K8" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -2716,10 +2716,10 @@
         <v>179500</v>
       </c>
       <c r="K9" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2751,10 +2751,10 @@
         <v>165000</v>
       </c>
       <c r="K10" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -2786,10 +2786,10 @@
         <v>135000</v>
       </c>
       <c r="K11" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -2821,10 +2821,10 @@
         <v>321500</v>
       </c>
       <c r="K12" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -2856,10 +2856,10 @@
         <v>186000</v>
       </c>
       <c r="K13" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2932,10 +2932,10 @@
         <v>20182805</v>
       </c>
       <c r="M15" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>236</v>
       </c>
@@ -2970,10 +2970,10 @@
         <v>20182786</v>
       </c>
       <c r="M16" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -3005,10 +3005,10 @@
         <v>270000</v>
       </c>
       <c r="K17" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3040,10 +3040,10 @@
         <v>223000</v>
       </c>
       <c r="K18" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -3078,10 +3078,10 @@
         <v>20182789</v>
       </c>
       <c r="M19" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -3113,10 +3113,10 @@
         <v>132000</v>
       </c>
       <c r="K20" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -3148,10 +3148,10 @@
         <v>51500</v>
       </c>
       <c r="K21" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>295</v>
       </c>
@@ -3186,10 +3186,10 @@
         <v>20182635</v>
       </c>
       <c r="M22" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>127</v>
       </c>
@@ -3221,10 +3221,10 @@
         <v>164500</v>
       </c>
       <c r="K23" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -3256,10 +3256,10 @@
         <v>860000</v>
       </c>
       <c r="K24" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -3297,10 +3297,10 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -3332,10 +3332,10 @@
         <v>95000</v>
       </c>
       <c r="K26" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>225</v>
       </c>
@@ -3367,10 +3367,10 @@
         <v>290000</v>
       </c>
       <c r="K27" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3405,10 +3405,10 @@
         <v>20182779</v>
       </c>
       <c r="M28" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3440,10 +3440,10 @@
         <v>91000</v>
       </c>
       <c r="K29" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>262</v>
       </c>
@@ -3475,10 +3475,10 @@
         <v>33000</v>
       </c>
       <c r="K30" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -3510,10 +3510,10 @@
         <v>747000</v>
       </c>
       <c r="K31" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -3545,10 +3545,10 @@
         <v>245000</v>
       </c>
       <c r="K32" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -3583,10 +3583,10 @@
         <v>20192924</v>
       </c>
       <c r="M33" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>112</v>
       </c>
@@ -3618,10 +3618,10 @@
         <v>376320</v>
       </c>
       <c r="K34" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -3653,10 +3653,10 @@
         <v>235000</v>
       </c>
       <c r="K35" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -3694,10 +3694,10 @@
         <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>290</v>
       </c>
@@ -3729,10 +3729,10 @@
         <v>139900</v>
       </c>
       <c r="K37" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -3767,10 +3767,10 @@
         <v>20182836</v>
       </c>
       <c r="M38" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>181</v>
       </c>
@@ -3805,10 +3805,10 @@
         <v>20182829</v>
       </c>
       <c r="M39" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -3840,10 +3840,10 @@
         <v>63000</v>
       </c>
       <c r="K40" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -3875,10 +3875,10 @@
         <v>98000</v>
       </c>
       <c r="K41" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -3910,10 +3910,10 @@
         <v>52500</v>
       </c>
       <c r="K42" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -3945,10 +3945,10 @@
         <v>117500</v>
       </c>
       <c r="K43" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -3980,10 +3980,10 @@
         <v>535000</v>
       </c>
       <c r="K44" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -4018,10 +4018,10 @@
         <v>20190037</v>
       </c>
       <c r="M45" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -4053,10 +4053,10 @@
         <v>48000</v>
       </c>
       <c r="K46" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>213</v>
       </c>
@@ -4088,10 +4088,10 @@
         <v>119900</v>
       </c>
       <c r="K47" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -4123,10 +4123,10 @@
         <v>159950</v>
       </c>
       <c r="K48" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>254</v>
       </c>
@@ -4158,10 +4158,10 @@
         <v>240000</v>
       </c>
       <c r="K49" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -4193,10 +4193,10 @@
         <v>135000</v>
       </c>
       <c r="K50" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -4234,10 +4234,10 @@
         <v>1</v>
       </c>
       <c r="M51" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -4269,10 +4269,10 @@
         <v>142000</v>
       </c>
       <c r="K52" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>288</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -4342,10 +4342,10 @@
         <v>132000</v>
       </c>
       <c r="K54" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -4377,10 +4377,10 @@
         <v>495000</v>
       </c>
       <c r="K55" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -4412,10 +4412,10 @@
         <v>155000</v>
       </c>
       <c r="K56" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -4447,10 +4447,10 @@
         <v>115000</v>
       </c>
       <c r="K57" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>343</v>
       </c>
@@ -4485,10 +4485,10 @@
         <v>20182761</v>
       </c>
       <c r="M58" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>139</v>
       </c>
@@ -4523,10 +4523,10 @@
         <v>20190030</v>
       </c>
       <c r="M59" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>162</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>140</v>
       </c>
@@ -4596,10 +4596,10 @@
         <v>530000</v>
       </c>
       <c r="K61" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -4631,10 +4631,10 @@
         <v>420000</v>
       </c>
       <c r="K62" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -4666,10 +4666,10 @@
         <v>150000</v>
       </c>
       <c r="K63" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -4701,10 +4701,10 @@
         <v>525000</v>
       </c>
       <c r="K64" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>154</v>
       </c>
@@ -4736,10 +4736,10 @@
         <v>191425</v>
       </c>
       <c r="K65" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>295</v>
       </c>
@@ -4774,10 +4774,10 @@
         <v>20182825</v>
       </c>
       <c r="M66" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -4809,10 +4809,10 @@
         <v>198000</v>
       </c>
       <c r="K67" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -4844,10 +4844,10 @@
         <v>265250</v>
       </c>
       <c r="K68" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>140</v>
       </c>
@@ -4879,10 +4879,10 @@
         <v>223000</v>
       </c>
       <c r="K69" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>185</v>
       </c>
@@ -4914,10 +4914,10 @@
         <v>27000</v>
       </c>
       <c r="K70" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -4949,10 +4949,10 @@
         <v>142900</v>
       </c>
       <c r="K71" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>259</v>
       </c>
@@ -4984,10 +4984,10 @@
         <v>50000</v>
       </c>
       <c r="K72" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -5019,10 +5019,10 @@
         <v>204500</v>
       </c>
       <c r="K73" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -5054,10 +5054,10 @@
         <v>133500</v>
       </c>
       <c r="K74" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -5095,10 +5095,10 @@
         <v>1</v>
       </c>
       <c r="M75" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>246</v>
       </c>
@@ -5130,10 +5130,10 @@
         <v>199900</v>
       </c>
       <c r="K76" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>51</v>
       </c>
@@ -5165,10 +5165,10 @@
         <v>299000</v>
       </c>
       <c r="K77" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -5206,10 +5206,10 @@
         <v>1</v>
       </c>
       <c r="M78" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -5241,10 +5241,10 @@
         <v>345000</v>
       </c>
       <c r="K79" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -5276,10 +5276,10 @@
         <v>50000</v>
       </c>
       <c r="K80" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>30</v>
       </c>
@@ -5311,10 +5311,10 @@
         <v>237500</v>
       </c>
       <c r="K81" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>154</v>
       </c>
@@ -5346,10 +5346,10 @@
         <v>369900</v>
       </c>
       <c r="K82" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -5381,10 +5381,10 @@
         <v>130000</v>
       </c>
       <c r="K83" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>59</v>
       </c>
@@ -5416,10 +5416,10 @@
         <v>189000</v>
       </c>
       <c r="K84" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>56</v>
       </c>
@@ -5457,10 +5457,10 @@
         <v>1</v>
       </c>
       <c r="M85" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -5495,10 +5495,10 @@
         <v>20182729</v>
       </c>
       <c r="M86" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>109</v>
       </c>
@@ -5530,10 +5530,10 @@
         <v>233000</v>
       </c>
       <c r="K87" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>60</v>
       </c>
@@ -5565,10 +5565,10 @@
         <v>307000</v>
       </c>
       <c r="K88" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>123</v>
       </c>
@@ -5600,10 +5600,10 @@
         <v>78000</v>
       </c>
       <c r="K89" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>53</v>
       </c>
@@ -5635,10 +5635,10 @@
         <v>370000</v>
       </c>
       <c r="K90" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -5673,10 +5673,10 @@
         <v>20182865</v>
       </c>
       <c r="M91" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>45</v>
       </c>
@@ -5708,10 +5708,10 @@
         <v>133000</v>
       </c>
       <c r="K92" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>402</v>
       </c>
@@ -5743,10 +5743,10 @@
         <v>133000</v>
       </c>
       <c r="K93" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>465</v>
       </c>
@@ -5781,10 +5781,10 @@
         <v>20182852</v>
       </c>
       <c r="M94" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>32</v>
       </c>
@@ -5816,10 +5816,10 @@
         <v>135000</v>
       </c>
       <c r="K95" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>294</v>
       </c>
@@ -5851,10 +5851,10 @@
         <v>274000</v>
       </c>
       <c r="K96" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>129</v>
       </c>
@@ -5889,10 +5889,10 @@
         <v>20182904</v>
       </c>
       <c r="M97" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -5924,10 +5924,10 @@
         <v>103000</v>
       </c>
       <c r="K98" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>75</v>
       </c>
@@ -5962,10 +5962,10 @@
         <v>20182817</v>
       </c>
       <c r="M99" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>73</v>
       </c>
@@ -5997,10 +5997,10 @@
         <v>280000</v>
       </c>
       <c r="K100" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>172</v>
       </c>
@@ -6032,10 +6032,10 @@
         <v>130000</v>
       </c>
       <c r="K101" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>78</v>
       </c>
@@ -6067,10 +6067,10 @@
         <v>112000</v>
       </c>
       <c r="K102" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>72</v>
       </c>
@@ -6102,10 +6102,10 @@
         <v>110100</v>
       </c>
       <c r="K103" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>168</v>
       </c>
@@ -6143,10 +6143,10 @@
         <v>1</v>
       </c>
       <c r="M104" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>53</v>
       </c>
@@ -6178,10 +6178,10 @@
         <v>310000</v>
       </c>
       <c r="K105" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>66</v>
       </c>
@@ -6216,10 +6216,10 @@
         <v>20182874</v>
       </c>
       <c r="M106" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -6254,10 +6254,10 @@
         <v>20182896</v>
       </c>
       <c r="M107" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>88</v>
       </c>
@@ -6295,10 +6295,10 @@
         <v>1</v>
       </c>
       <c r="M108" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -6333,10 +6333,10 @@
         <v>20190072</v>
       </c>
       <c r="M109" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>183</v>
       </c>
@@ -6368,10 +6368,10 @@
         <v>145000</v>
       </c>
       <c r="K110" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>74</v>
       </c>
@@ -6403,10 +6403,10 @@
         <v>78000</v>
       </c>
       <c r="K111" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>176</v>
       </c>
@@ -6438,10 +6438,10 @@
         <v>176900</v>
       </c>
       <c r="K112" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>32</v>
       </c>
@@ -6473,10 +6473,10 @@
         <v>30000</v>
       </c>
       <c r="K113" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>126</v>
       </c>
@@ -6511,10 +6511,10 @@
         <v>20192925</v>
       </c>
       <c r="M114" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>127</v>
       </c>
@@ -6545,11 +6545,8 @@
       <c r="J115" s="2">
         <v>88400</v>
       </c>
-      <c r="K115" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>34</v>
       </c>
@@ -6580,17 +6577,8 @@
       <c r="J116" s="2">
         <v>158400</v>
       </c>
-      <c r="K116">
-        <v>20182854</v>
-      </c>
-      <c r="L116" t="b">
-        <v>1</v>
-      </c>
-      <c r="M116" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>67</v>
       </c>
@@ -6621,11 +6609,8 @@
       <c r="J117" s="2">
         <v>290000</v>
       </c>
-      <c r="K117" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>79</v>
       </c>
@@ -6656,11 +6641,8 @@
       <c r="J118" s="2">
         <v>180000</v>
       </c>
-      <c r="K118" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>53</v>
       </c>
@@ -6691,11 +6673,8 @@
       <c r="J119" s="2">
         <v>80000</v>
       </c>
-      <c r="K119" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>186</v>
       </c>
@@ -6726,11 +6705,8 @@
       <c r="J120" s="2">
         <v>75000</v>
       </c>
-      <c r="K120" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>190</v>
       </c>
@@ -6761,11 +6737,8 @@
       <c r="J121" s="2">
         <v>184900</v>
       </c>
-      <c r="K121" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -6796,11 +6769,8 @@
       <c r="J122" s="2">
         <v>405000</v>
       </c>
-      <c r="K122" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>34</v>
       </c>
@@ -6831,11 +6801,8 @@
       <c r="J123" s="2">
         <v>273000</v>
       </c>
-      <c r="K123" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>289</v>
       </c>
@@ -6866,11 +6833,8 @@
       <c r="J124" s="2">
         <v>43750</v>
       </c>
-      <c r="K124" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>50</v>
       </c>
@@ -6901,11 +6865,8 @@
       <c r="J125" s="2">
         <v>179000</v>
       </c>
-      <c r="K125" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>35</v>
       </c>
@@ -6935,9 +6896,6 @@
       </c>
       <c r="J126" s="2">
         <v>232000</v>
-      </c>
-      <c r="K126" t="s">
-        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted multithreading to Parallel.For loop; cleaned up code
</commit_message>
<xml_diff>
--- a/Testing Files/Determiner Test Files/HatcoMLSDataTestingSmall.xlsx
+++ b/Testing Files/Determiner Test Files/HatcoMLSDataTestingSmall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\HatcoMarketShareHelper\Testing Files\Determiner Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0102E18F-7F87-49B8-9931-430C03D888E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D579F329-2C7A-4B25-9891-8C08A9248E09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="498">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -1506,10 +1506,10 @@
     <t>Escrow Officer</t>
   </si>
   <si>
+    <t>did not close</t>
+  </si>
+  <si>
     <t>Tiffany Minnish</t>
-  </si>
-  <si>
-    <t>did not close</t>
   </si>
   <si>
     <t>Phyllis Alexander</t>
@@ -2371,7 +2371,7 @@
   <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,7 +2456,7 @@
         <v>135750</v>
       </c>
       <c r="K2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>20182762</v>
       </c>
       <c r="M4" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2570,7 +2570,7 @@
         <v>365000</v>
       </c>
       <c r="K5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2646,7 +2646,7 @@
         <v>86500</v>
       </c>
       <c r="K7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2681,7 +2681,7 @@
         <v>151800</v>
       </c>
       <c r="K8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2716,7 +2716,7 @@
         <v>179500</v>
       </c>
       <c r="K9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>165000</v>
       </c>
       <c r="K10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2786,7 +2786,7 @@
         <v>135000</v>
       </c>
       <c r="K11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2821,7 +2821,7 @@
         <v>321500</v>
       </c>
       <c r="K12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2856,7 +2856,7 @@
         <v>186000</v>
       </c>
       <c r="K13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
         <v>20182786</v>
       </c>
       <c r="M16" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3005,7 +3005,7 @@
         <v>270000</v>
       </c>
       <c r="K17" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>223000</v>
       </c>
       <c r="K18" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -3113,7 +3113,7 @@
         <v>132000</v>
       </c>
       <c r="K20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>51500</v>
       </c>
       <c r="K21" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -3221,7 +3221,7 @@
         <v>164500</v>
       </c>
       <c r="K23" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -3256,7 +3256,7 @@
         <v>860000</v>
       </c>
       <c r="K24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3332,7 +3332,7 @@
         <v>95000</v>
       </c>
       <c r="K26" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -3367,7 +3367,7 @@
         <v>290000</v>
       </c>
       <c r="K27" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -3440,7 +3440,7 @@
         <v>91000</v>
       </c>
       <c r="K29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -3475,7 +3475,7 @@
         <v>33000</v>
       </c>
       <c r="K30" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3510,7 +3510,7 @@
         <v>747000</v>
       </c>
       <c r="K31" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3545,7 +3545,7 @@
         <v>245000</v>
       </c>
       <c r="K32" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -3618,7 +3618,7 @@
         <v>376320</v>
       </c>
       <c r="K34" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -3653,7 +3653,7 @@
         <v>235000</v>
       </c>
       <c r="K35" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -3729,7 +3729,7 @@
         <v>139900</v>
       </c>
       <c r="K37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -3840,7 +3840,7 @@
         <v>63000</v>
       </c>
       <c r="K40" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3875,7 +3875,7 @@
         <v>98000</v>
       </c>
       <c r="K41" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3910,7 +3910,7 @@
         <v>52500</v>
       </c>
       <c r="K42" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3945,7 +3945,7 @@
         <v>117500</v>
       </c>
       <c r="K43" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3980,7 +3980,7 @@
         <v>535000</v>
       </c>
       <c r="K44" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
         <v>48000</v>
       </c>
       <c r="K46" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -4088,7 +4088,7 @@
         <v>119900</v>
       </c>
       <c r="K47" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -4123,7 +4123,7 @@
         <v>159950</v>
       </c>
       <c r="K48" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -4158,7 +4158,7 @@
         <v>240000</v>
       </c>
       <c r="K49" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -4193,7 +4193,7 @@
         <v>135000</v>
       </c>
       <c r="K50" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -4269,7 +4269,7 @@
         <v>142000</v>
       </c>
       <c r="K52" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -4342,7 +4342,7 @@
         <v>132000</v>
       </c>
       <c r="K54" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -4377,7 +4377,7 @@
         <v>495000</v>
       </c>
       <c r="K55" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -4412,7 +4412,7 @@
         <v>155000</v>
       </c>
       <c r="K56" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -4447,7 +4447,7 @@
         <v>115000</v>
       </c>
       <c r="K57" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>530000</v>
       </c>
       <c r="K61" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -4631,7 +4631,7 @@
         <v>420000</v>
       </c>
       <c r="K62" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -4666,7 +4666,7 @@
         <v>150000</v>
       </c>
       <c r="K63" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -4701,7 +4701,7 @@
         <v>525000</v>
       </c>
       <c r="K64" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -4736,7 +4736,7 @@
         <v>191425</v>
       </c>
       <c r="K65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -4809,7 +4809,7 @@
         <v>198000</v>
       </c>
       <c r="K67" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>265250</v>
       </c>
       <c r="K68" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -4879,7 +4879,7 @@
         <v>223000</v>
       </c>
       <c r="K69" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -4914,7 +4914,7 @@
         <v>27000</v>
       </c>
       <c r="K70" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -4949,7 +4949,7 @@
         <v>142900</v>
       </c>
       <c r="K71" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -4984,7 +4984,7 @@
         <v>50000</v>
       </c>
       <c r="K72" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -5019,7 +5019,7 @@
         <v>204500</v>
       </c>
       <c r="K73" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -5054,7 +5054,7 @@
         <v>133500</v>
       </c>
       <c r="K74" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -5130,7 +5130,7 @@
         <v>199900</v>
       </c>
       <c r="K76" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -5165,7 +5165,7 @@
         <v>299000</v>
       </c>
       <c r="K77" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>345000</v>
       </c>
       <c r="K79" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -5276,7 +5276,7 @@
         <v>50000</v>
       </c>
       <c r="K80" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -5311,7 +5311,7 @@
         <v>237500</v>
       </c>
       <c r="K81" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -5346,7 +5346,7 @@
         <v>369900</v>
       </c>
       <c r="K82" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -5381,7 +5381,7 @@
         <v>130000</v>
       </c>
       <c r="K83" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -5416,7 +5416,7 @@
         <v>189000</v>
       </c>
       <c r="K84" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -5530,7 +5530,7 @@
         <v>233000</v>
       </c>
       <c r="K87" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -5565,7 +5565,7 @@
         <v>307000</v>
       </c>
       <c r="K88" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -5600,7 +5600,7 @@
         <v>78000</v>
       </c>
       <c r="K89" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -5635,7 +5635,7 @@
         <v>370000</v>
       </c>
       <c r="K90" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -5708,7 +5708,7 @@
         <v>133000</v>
       </c>
       <c r="K92" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -5743,7 +5743,7 @@
         <v>133000</v>
       </c>
       <c r="K93" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -5781,7 +5781,7 @@
         <v>20182852</v>
       </c>
       <c r="M94" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -5816,7 +5816,7 @@
         <v>135000</v>
       </c>
       <c r="K95" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -5851,7 +5851,7 @@
         <v>274000</v>
       </c>
       <c r="K96" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -5924,7 +5924,7 @@
         <v>103000</v>
       </c>
       <c r="K98" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -5997,7 +5997,7 @@
         <v>280000</v>
       </c>
       <c r="K100" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -6032,7 +6032,7 @@
         <v>130000</v>
       </c>
       <c r="K101" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -6067,7 +6067,7 @@
         <v>112000</v>
       </c>
       <c r="K102" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -6102,7 +6102,7 @@
         <v>110100</v>
       </c>
       <c r="K103" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -6178,7 +6178,7 @@
         <v>310000</v>
       </c>
       <c r="K105" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -6368,7 +6368,7 @@
         <v>145000</v>
       </c>
       <c r="K110" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -6403,7 +6403,7 @@
         <v>78000</v>
       </c>
       <c r="K111" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -6438,7 +6438,7 @@
         <v>176900</v>
       </c>
       <c r="K112" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -6473,7 +6473,7 @@
         <v>30000</v>
       </c>
       <c r="K113" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -6545,6 +6545,9 @@
       <c r="J115" s="2">
         <v>88400</v>
       </c>
+      <c r="K115" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
@@ -6577,6 +6580,15 @@
       <c r="J116" s="2">
         <v>158400</v>
       </c>
+      <c r="K116">
+        <v>20182854</v>
+      </c>
+      <c r="L116" t="b">
+        <v>1</v>
+      </c>
+      <c r="M116" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -6609,6 +6621,9 @@
       <c r="J117" s="2">
         <v>290000</v>
       </c>
+      <c r="K117" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -6641,6 +6656,9 @@
       <c r="J118" s="2">
         <v>180000</v>
       </c>
+      <c r="K118" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -6673,6 +6691,9 @@
       <c r="J119" s="2">
         <v>80000</v>
       </c>
+      <c r="K119" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
@@ -6705,6 +6726,9 @@
       <c r="J120" s="2">
         <v>75000</v>
       </c>
+      <c r="K120" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
@@ -6737,6 +6761,9 @@
       <c r="J121" s="2">
         <v>184900</v>
       </c>
+      <c r="K121" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -6769,6 +6796,9 @@
       <c r="J122" s="2">
         <v>405000</v>
       </c>
+      <c r="K122" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -6801,6 +6831,9 @@
       <c r="J123" s="2">
         <v>273000</v>
       </c>
+      <c r="K123" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -6833,6 +6866,9 @@
       <c r="J124" s="2">
         <v>43750</v>
       </c>
+      <c r="K124" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -6865,6 +6901,9 @@
       <c r="J125" s="2">
         <v>179000</v>
       </c>
+      <c r="K125" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -6896,6 +6935,9 @@
       </c>
       <c r="J126" s="2">
         <v>232000</v>
+      </c>
+      <c r="K126" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>